<commit_message>
Utf-8 pour plug in
</commit_message>
<xml_diff>
--- a/CatalogueProduits.xlsx
+++ b/CatalogueProduits.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
     <t>Description</t>
   </si>
@@ -223,9 +223,6 @@
     <t>20x30cm_WANTED</t>
   </si>
   <si>
-    <t>10x15cm_CADRE-CARRE-ID-FBI</t>
-  </si>
-  <si>
     <t>Affiche Wanted</t>
   </si>
   <si>
@@ -332,6 +329,15 @@
   </si>
   <si>
     <t>18x22cm_INSITU-VOEUX</t>
+  </si>
+  <si>
+    <t>Affiche Undesirable</t>
+  </si>
+  <si>
+    <t>20x30cm_UNDESIRABLE</t>
+  </si>
+  <si>
+    <t>10x15cm_CADRE-FBI-IDENTITE</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1343024</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -809,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,161 +1037,191 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
+        <f>'Gen Catalog'!E22</f>
+        <v>Produits Carrés Cadre-ID</v>
+      </c>
+      <c r="B22" t="str">
+        <f>'Gen Catalog'!F22</f>
+        <v>18x18cm_CADRE-CARRE-ID</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
         <f>'Gen Catalog'!E23</f>
         <v>Produits Carrés In Situ-ID</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B23" t="str">
         <f>'Gen Catalog'!F23</f>
         <v>18x18cm_INSITU-CARRE-ID</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
         <f>'Gen Catalog'!E24</f>
         <v>Noir &amp; Blanc Carré N&amp;B 18 cm</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B24" t="str">
         <f>'Gen Catalog'!F24</f>
         <v>18x18cm_PORTRAIT_NOIR-ET-BLANC</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
         <f>'Gen Catalog'!E25</f>
         <v>Noir &amp; Blanc Carré N&amp;B 30 cm</v>
       </c>
-      <c r="B24" t="str">
+      <c r="B25" t="str">
         <f>'Gen Catalog'!F25</f>
         <v>30x30cm_PORTRAIT_NOIR-ET-BLANC</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
         <f>'Gen Catalog'!E26</f>
         <v>Pour les enfants Carte de FBI</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B26" t="str">
         <f>'Gen Catalog'!F26</f>
-        <v>10x15cm_CADRE-CARRE-ID-FBI</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+        <v>10x15cm_CADRE-FBI-IDENTITE</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>'Gen Catalog'!E27</f>
+        <v>Calendriers &amp; Voeux C - 4 Cartes de Voeux</v>
+      </c>
+      <c r="B27" t="str">
+        <f>'Gen Catalog'!F27</f>
+        <v>18x22cm_CADRE-VOEUX</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
         <f>'Gen Catalog'!E28</f>
         <v>Calendriers &amp; Voeux I - 4 Cartes de Voeux</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B28" t="str">
         <f>'Gen Catalog'!F28</f>
         <v>18x22cm_INSITU-VOEUX</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
         <f>'Gen Catalog'!E29</f>
         <v>Pour les enfants Affiche Wanted</v>
       </c>
-      <c r="B27" t="str">
+      <c r="B29" t="str">
         <f>'Gen Catalog'!F29</f>
         <v>20x30cm_WANTED</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f>'Gen Catalog'!E30</f>
-        <v>STANDARD MB STANDARD MB</v>
-      </c>
-      <c r="B28">
-        <f>'Gen Catalog'!F30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f>'Gen Catalog'!E31</f>
-        <v>Photo de classe Groupe classe 18x24cm</v>
-      </c>
-      <c r="B29" t="str">
-        <f>'Gen Catalog'!F31</f>
-        <v>18x24cm_TRAD</v>
-      </c>
-    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>'Gen Catalog'!E32</f>
-        <v>Agrandissements 10x15 cm</v>
+        <f>'Gen Catalog'!E30</f>
+        <v>Pour les enfants Affiche Undesirable</v>
       </c>
       <c r="B30" t="str">
-        <f>'Gen Catalog'!F32</f>
-        <v>10x15cm_PORTRAIT</v>
+        <f>'Gen Catalog'!F30</f>
+        <v>20x30cm_UNDESIRABLE</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>'Gen Catalog'!E33</f>
-        <v>Agrandissements 15x23 cm</v>
-      </c>
-      <c r="B31" t="str">
-        <f>'Gen Catalog'!F33</f>
-        <v>15x23cm_PORTRAIT</v>
+        <f>'Gen Catalog'!E31</f>
+        <v>STANDARD MB STANDARD MB</v>
+      </c>
+      <c r="B31">
+        <f>'Gen Catalog'!F31</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>'Gen Catalog'!E34</f>
-        <v>Agrandissements 20x30 cm</v>
+        <f>'Gen Catalog'!E32</f>
+        <v>Photo de classe Groupe classe 18x24cm</v>
       </c>
       <c r="B32" t="str">
-        <f>'Gen Catalog'!F34</f>
-        <v>20x30cm_PORTRAIT</v>
+        <f>'Gen Catalog'!F32</f>
+        <v>18x24cm_TRAD</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>'Gen Catalog'!E35</f>
-        <v>Produits Calendrier avec photo 20x30 cm</v>
+        <f>'Gen Catalog'!E33</f>
+        <v>Agrandissements 10x15 cm</v>
       </c>
       <c r="B33" t="str">
-        <f>'Gen Catalog'!F35</f>
-        <v>20x30cm_CAL-INDIV</v>
+        <f>'Gen Catalog'!F33</f>
+        <v>10x15cm_PORTRAIT</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>'Gen Catalog'!E36</f>
-        <v>Produits Calendrier avec groupe 20x30 cm</v>
+        <f>'Gen Catalog'!E34</f>
+        <v>Agrandissements 15x23 cm</v>
       </c>
       <c r="B34" t="str">
-        <f>'Gen Catalog'!F36</f>
-        <v>20x30cm_CAL-TRAD</v>
+        <f>'Gen Catalog'!F34</f>
+        <v>15x23cm_PORTRAIT</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>'Gen Catalog'!E37</f>
-        <v>Produits 8 Photos identitées</v>
+        <f>'Gen Catalog'!E35</f>
+        <v>Agrandissements 20x30 cm</v>
       </c>
       <c r="B35" t="str">
-        <f>'Gen Catalog'!F37</f>
-        <v>10x15cm_8xID</v>
+        <f>'Gen Catalog'!F35</f>
+        <v>20x30cm_PORTRAIT</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>'Gen Catalog'!E38</f>
-        <v>Produits Duo 10x15 cm</v>
+        <f>'Gen Catalog'!E36</f>
+        <v>Produits Calendrier avec photo 20x30 cm</v>
       </c>
       <c r="B36" t="str">
-        <f>'Gen Catalog'!F38</f>
-        <v>15x23cm_DUO-DIX-QUINZE</v>
+        <f>'Gen Catalog'!F36</f>
+        <v>20x30cm_CAL-INDIV</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
+        <f>'Gen Catalog'!E37</f>
+        <v>Produits Calendrier avec groupe 20x30 cm</v>
+      </c>
+      <c r="B37" t="str">
+        <f>'Gen Catalog'!F37</f>
+        <v>20x30cm_CAL-TRAD</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>'Gen Catalog'!E38</f>
+        <v>Produits 8 Photos identitées</v>
+      </c>
+      <c r="B38" t="str">
+        <f>'Gen Catalog'!F38</f>
+        <v>10x15cm_8xID</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
         <f>'Gen Catalog'!E39</f>
+        <v>Produits Duo 10x15 cm</v>
+      </c>
+      <c r="B39" t="str">
+        <f>'Gen Catalog'!F39</f>
+        <v>15x23cm_DUO-DIX-QUINZE</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>'Gen Catalog'!E40</f>
         <v>Produits Double 10x15 cm</v>
       </c>
-      <c r="B37" t="str">
-        <f>'Gen Catalog'!F39</f>
+      <c r="B40" t="str">
+        <f>'Gen Catalog'!F40</f>
         <v>15x23cm_DIX-QUINZE</v>
       </c>
     </row>
@@ -1197,11 +1233,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,22 +1253,22 @@
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>0</v>
@@ -1477,7 +1513,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ref="E14:E40" si="2">A14 &amp; " " &amp; B14</f>
+        <f t="shared" ref="E14:E41" si="2">A14 &amp; " " &amp; B14</f>
         <v>Agrandissements Carrés Carré 18 cm</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1651,14 +1687,14 @@
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="2"/>
         <v>Produits Carrés In Situ-ID</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1688,7 +1724,7 @@
         <v>Noir &amp; Blanc Carré N&amp;B 30 cm</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1703,7 +1739,7 @@
         <v>Pour les enfants Carte de FBI</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1711,7 +1747,7 @@
         <v>57</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" ref="E27" si="4">A27 &amp; " " &amp; B27</f>
@@ -1726,14 +1762,14 @@
         <v>57</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="2"/>
         <v>Calendriers &amp; Voeux I - 4 Cartes de Voeux</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1741,7 +1777,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="2"/>
@@ -1751,221 +1787,236 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" ref="E30" si="5">A30 &amp; " " &amp; B30</f>
+        <v>Pour les enfants Affiche Undesirable</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>STANDARD MB STANDARD MB</v>
+      </c>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>STANDARD MB STANDARD MB</v>
-      </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" t="str">
+      <c r="C32" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="str">
         <f t="shared" si="2"/>
         <v>Photo de classe Groupe classe 18x24cm</v>
       </c>
-      <c r="F31" s="1" t="str">
-        <f>C31&amp;"_"&amp;D31</f>
+      <c r="F32" s="1" t="str">
+        <f>C32&amp;"_"&amp;D32</f>
         <v>18x24cm_TRAD</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="2"/>
-        <v>Agrandissements 10x15 cm</v>
-      </c>
-      <c r="F32" s="1" t="str">
-        <f t="shared" ref="F32:F39" si="5">C32&amp;"_"&amp;D32</f>
-        <v>10x15cm_PORTRAIT</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="2"/>
-        <v>Agrandissements 15x23 cm</v>
+        <v>Agrandissements 10x15 cm</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>15x23cm_PORTRAIT</v>
+        <f t="shared" ref="F33:F40" si="6">C33&amp;"_"&amp;D33</f>
+        <v>10x15cm_PORTRAIT</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="2"/>
-        <v>Agrandissements 20x30 cm</v>
+        <v>Agrandissements 15x23 cm</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>20x30cm_PORTRAIT</v>
+        <f t="shared" si="6"/>
+        <v>15x23cm_PORTRAIT</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="2"/>
-        <v>Produits Calendrier avec photo 20x30 cm</v>
+        <v>Agrandissements 20x30 cm</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>20x30cm_CAL-INDIV</v>
+        <f t="shared" si="6"/>
+        <v>20x30cm_PORTRAIT</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="2"/>
-        <v>Produits Calendrier avec groupe 20x30 cm</v>
+        <v>Produits Calendrier avec photo 20x30 cm</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>20x30cm_CAL-TRAD</v>
+        <f t="shared" si="6"/>
+        <v>20x30cm_CAL-INDIV</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="2"/>
-        <v>Produits 8 Photos identitées</v>
+        <v>Produits Calendrier avec groupe 20x30 cm</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>10x15cm_8xID</v>
+        <f t="shared" si="6"/>
+        <v>20x30cm_CAL-TRAD</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="2"/>
-        <v>Produits Duo 10x15 cm</v>
+        <v>Produits 8 Photos identitées</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>15x23cm_DUO-DIX-QUINZE</v>
+        <f t="shared" si="6"/>
+        <v>10x15cm_8xID</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="2"/>
+        <v>Produits Duo 10x15 cm</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>15x23cm_DUO-DIX-QUINZE</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
         <v>Produits Double 10x15 cm</v>
       </c>
-      <c r="F39" s="1" t="str">
-        <f t="shared" si="5"/>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>15x23cm_DIX-QUINZE</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E40" t="str">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>

</xml_diff>